<commit_message>
Nå begynner det å komme seg
</commit_message>
<xml_diff>
--- a/data/Ormset_Data.xlsx
+++ b/data/Ormset_Data.xlsx
@@ -86,7 +86,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,12 +97,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -134,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -161,9 +155,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -480,9 +471,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -617,25 +608,25 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <v>0</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <v>0</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <v>1.6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Scenario based topology model
</commit_message>
<xml_diff>
--- a/data/Ormset_Data.xlsx
+++ b/data/Ormset_Data.xlsx
@@ -89,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,12 +100,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -137,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -151,11 +145,8 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -164,9 +155,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -486,19 +474,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -506,10 +494,10 @@
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="10">
         <v>45</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="10">
         <v>20</v>
       </c>
     </row>
@@ -517,10 +505,10 @@
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
+      <c r="B3" s="10">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10">
         <v>0</v>
       </c>
     </row>
@@ -528,10 +516,10 @@
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="10">
         <v>45</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="10">
         <v>20</v>
       </c>
     </row>
@@ -539,10 +527,10 @@
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="12">
-        <v>388</v>
-      </c>
-      <c r="C5" s="12">
+      <c r="B5" s="10">
+        <v>389</v>
+      </c>
+      <c r="C5" s="10">
         <v>331.5</v>
       </c>
     </row>
@@ -550,10 +538,10 @@
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="10">
         <v>375</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="10">
         <v>326</v>
       </c>
     </row>
@@ -561,32 +549,32 @@
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="12">
-        <v>388</v>
-      </c>
-      <c r="C7" s="12">
-        <v>331</v>
+      <c r="B7" s="10">
+        <v>389</v>
+      </c>
+      <c r="C7" s="10">
+        <v>331.5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="12">
-        <v>2</v>
-      </c>
-      <c r="C8" s="12">
-        <v>2</v>
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="10">
         <v>12</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="10">
         <v>12</v>
       </c>
     </row>
@@ -594,10 +582,10 @@
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="12">
-        <v>0</v>
-      </c>
-      <c r="C10" s="12">
+      <c r="B10" s="10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="10">
         <v>0</v>
       </c>
     </row>
@@ -605,10 +593,10 @@
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="10">
         <v>43</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="10">
         <v>30</v>
       </c>
     </row>
@@ -616,10 +604,10 @@
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="10">
         <v>4</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="10">
         <v>2</v>
       </c>
     </row>
@@ -627,10 +615,10 @@
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="12">
-        <v>0</v>
-      </c>
-      <c r="C13" s="12">
+      <c r="B13" s="10">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10">
         <v>0</v>
       </c>
     </row>
@@ -638,10 +626,10 @@
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="12">
-        <v>0</v>
-      </c>
-      <c r="C14" s="12">
+      <c r="B14" s="10">
+        <v>0</v>
+      </c>
+      <c r="C14" s="10">
         <v>1.6</v>
       </c>
     </row>
@@ -661,15 +649,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="16.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="16.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="17.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -889,12 +877,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="10.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -949,14 +937,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -967,7 +955,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -978,7 +966,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4">
         <v>1.667</v>
       </c>
@@ -989,7 +977,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4">
         <v>3.4</v>
       </c>
@@ -1000,7 +988,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4">
         <v>4.2</v>
       </c>
@@ -1011,7 +999,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4">
         <v>5.1</v>
       </c>
@@ -1022,7 +1010,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4">
         <v>7.1</v>
       </c>
@@ -1033,7 +1021,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4">
         <v>9.2</v>
       </c>
@@ -1044,7 +1032,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4">
         <v>11.4</v>
       </c>
@@ -1055,7 +1043,7 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3">
         <v>13.7</v>
       </c>
@@ -1066,7 +1054,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4">
         <v>16.4</v>
       </c>
@@ -1077,7 +1065,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="4">
         <v>18.8</v>
       </c>
@@ -1088,7 +1076,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4">
         <v>20</v>
       </c>
@@ -1099,9 +1087,9 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">

</xml_diff>

<commit_message>
updated start volumes and load to 0.00175
</commit_message>
<xml_diff>
--- a/data/Ormset_Data.xlsx
+++ b/data/Ormset_Data.xlsx
@@ -523,10 +523,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="10">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C4" s="10">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">

</xml_diff>